<commit_message>
Fixing completion Order bug and tweak order timing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,28 +3,34 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="37245" yWindow="1020" windowWidth="21600" windowHeight="13830" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="31875" yWindow="1380" windowWidth="21600" windowHeight="13830" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10 second wait for orders" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -38,12 +44,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -56,9 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -460,7 +484,7 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -476,10 +500,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -530,19 +554,24 @@
           <t>3-Star</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Total Customers</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.04</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
         <v>36</v>
       </c>
       <c r="D2" t="n">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -558,6 +587,9 @@
       </c>
       <c r="I2" t="n">
         <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -565,13 +597,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>21.14</v>
+        <v>22.46</v>
       </c>
       <c r="C3" t="n">
         <v>36</v>
       </c>
       <c r="D3" t="n">
-        <v>569</v>
+        <v>591</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -587,6 +619,9 @@
       </c>
       <c r="I3" t="n">
         <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -594,19 +629,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>32.78</v>
+        <v>33.62</v>
       </c>
       <c r="C4" t="n">
         <v>36</v>
       </c>
       <c r="D4" t="n">
-        <v>963</v>
+        <v>917</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -616,6 +651,9 @@
       </c>
       <c r="I4" t="n">
         <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -623,13 +661,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>47.18</v>
+        <v>47.66</v>
       </c>
       <c r="C5" t="n">
         <v>36</v>
       </c>
       <c r="D5" t="n">
-        <v>1453</v>
+        <v>1461</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
@@ -645,6 +683,9 @@
       </c>
       <c r="I5" t="n">
         <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -652,16 +693,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>57.44</v>
+        <v>111.58</v>
       </c>
       <c r="C6" t="n">
         <v>36</v>
       </c>
       <c r="D6" t="n">
-        <v>1.844</v>
+        <v>1943</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
         <v>13</v>
@@ -674,6 +715,9 @@
       </c>
       <c r="I6" t="n">
         <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -681,16 +725,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>151.78</v>
+        <v>165.32</v>
       </c>
       <c r="C7" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="n">
-        <v>24332</v>
+        <v>2422</v>
       </c>
       <c r="E7" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>15</v>
@@ -703,6 +747,9 @@
       </c>
       <c r="I7" t="n">
         <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -710,28 +757,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>242.24</v>
+        <v>219.96</v>
       </c>
       <c r="C8" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>3.018</v>
+        <v>2916</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -739,13 +789,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>180.28</v>
+        <v>179.64</v>
       </c>
       <c r="C9" t="n">
         <v>33</v>
       </c>
       <c r="D9" t="n">
-        <v>3635</v>
+        <v>3582</v>
       </c>
       <c r="E9" t="n">
         <v>6</v>
@@ -761,6 +811,9 @@
       </c>
       <c r="I9" t="n">
         <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -768,19 +821,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>71.90000000000001</v>
+        <v>69.84</v>
       </c>
       <c r="C10" t="n">
         <v>29</v>
       </c>
       <c r="D10" t="n">
-        <v>4.254</v>
+        <v>4164</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -790,6 +843,9 @@
       </c>
       <c r="I10" t="n">
         <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -797,28 +853,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>141.74</v>
+        <v>142.34</v>
       </c>
       <c r="C11" t="n">
         <v>27</v>
       </c>
       <c r="D11" t="n">
-        <v>4.875</v>
+        <v>4934</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F11" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1470,4 +1529,395 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Money</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Shop Items Remaining</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Customer Points</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>0-Star</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>1-Star</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>2-Star</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>3-Star</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Total Customers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5.94</v>
+      </c>
+      <c r="C2" t="n">
+        <v>36</v>
+      </c>
+      <c r="D2" t="n">
+        <v>199</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>22.34</v>
+      </c>
+      <c r="C3" t="n">
+        <v>36</v>
+      </c>
+      <c r="D3" t="n">
+        <v>589</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>34.04</v>
+      </c>
+      <c r="C4" t="n">
+        <v>36</v>
+      </c>
+      <c r="D4" t="n">
+        <v>984</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>48.14</v>
+      </c>
+      <c r="C5" t="n">
+        <v>36</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1469</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>112.12</v>
+      </c>
+      <c r="C6" t="n">
+        <v>36</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1952</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>106.28</v>
+      </c>
+      <c r="C7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2438</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>220.08</v>
+      </c>
+      <c r="C8" t="n">
+        <v>34</v>
+      </c>
+      <c r="D8" t="n">
+        <v>29118</v>
+      </c>
+      <c r="E8" t="n">
+        <v>19</v>
+      </c>
+      <c r="F8" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>32</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3406</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>17</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>115.9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>29</v>
+      </c>
+      <c r="D10" t="n">
+        <v>181</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>16</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>148.1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>27</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5149</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrections to overlay and added overlay to main
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10 second wait for orders" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1920,4 +1921,235 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Money</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Shop Items Remaining</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Customer Points</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>0-Star</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>1-Star</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>2-Star</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>3-Star</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Total Customers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>55.94</v>
+      </c>
+      <c r="C2" t="n">
+        <v>36</v>
+      </c>
+      <c r="D2" t="n">
+        <v>199</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>522.28</v>
+      </c>
+      <c r="C3" t="n">
+        <v>36</v>
+      </c>
+      <c r="D3" t="n">
+        <v>588</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>515.92</v>
+      </c>
+      <c r="C4" t="n">
+        <v>27</v>
+      </c>
+      <c r="D4" t="n">
+        <v>982</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>530.08</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1468</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>576.42</v>
+      </c>
+      <c r="C6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1957</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>